<commit_message>
adding ability to save schenario result
</commit_message>
<xml_diff>
--- a/src/main/java/framework/suites/regression/OSPOS_Automation_Test_Case.xlsx
+++ b/src/main/java/framework/suites/regression/OSPOS_Automation_Test_Case.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nazmul.islam/Desktop/Personal/HyperTech/ht-selenium-framework/src/main/java/framework/suite/regression/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nazmul.islam/Desktop/Personal/HyperTech/ht-selenium-framework/src/main/java/framework/suites/regression/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02362C20-5698-7246-88CB-B0A438FBB76A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{862A37D3-2A83-5B49-B095-49450BBB746F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="14540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="14540" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TS" sheetId="1" r:id="rId1"/>
@@ -135,9 +135,6 @@
     <t>#title_bar &gt; button:nth-child(2)</t>
   </si>
   <si>
-    <t>first_name</t>
-  </si>
-  <si>
     <t>Nazmul</t>
   </si>
   <si>
@@ -151,6 +148,9 @@
   </si>
   <si>
     <t>submit</t>
+  </si>
+  <si>
+    <t>first_name</t>
   </si>
 </sst>
 </file>
@@ -574,7 +574,7 @@
   </sheetPr>
   <dimension ref="A1:Z102"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
@@ -3488,8 +3488,8 @@
   </sheetPr>
   <dimension ref="A1:Z100"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -3786,10 +3786,10 @@
         <v>20</v>
       </c>
       <c r="E9" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="F9" s="4" t="s">
         <v>37</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>38</v>
       </c>
       <c r="G9" s="9"/>
       <c r="H9" s="9"/>
@@ -3824,10 +3824,10 @@
         <v>20</v>
       </c>
       <c r="E10" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="F10" s="4" t="s">
         <v>39</v>
-      </c>
-      <c r="F10" s="4" t="s">
-        <v>40</v>
       </c>
       <c r="G10" s="9"/>
       <c r="H10" s="9"/>
@@ -3859,10 +3859,10 @@
         <v>27</v>
       </c>
       <c r="D11" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="E11" s="4" t="s">
         <v>41</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>42</v>
       </c>
       <c r="F11" s="9"/>
       <c r="G11" s="9"/>

</xml_diff>